<commit_message>
Add "Upload data" module tutorial
</commit_message>
<xml_diff>
--- a/text/tutorials/Tutoriales_introJS.xlsx
+++ b/text/tutorials/Tutoriales_introJS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carles/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RDynamics/R_folder/relconfig/text/tutorials/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="20960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="page_generator" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>step</t>
   </si>
@@ -67,21 +67,12 @@
     <t>#page_generator-tut_scale</t>
   </si>
   <si>
-    <t>#page_generator-</t>
-  </si>
-  <si>
     <t>Text</t>
   </si>
   <si>
     <t>#page_generator-tut_confinter</t>
   </si>
   <si>
-    <t>#page_generator-countour_plot</t>
-  </si>
-  <si>
-    <t>#page_generator-legendPlot</t>
-  </si>
-  <si>
     <t>#page_generator-intro</t>
   </si>
   <si>
@@ -113,12 +104,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a generic welcome message, press the buttons below the navigate trough the elements of this page. This is a generic welcome message, press the buttons below the navigate trough the elements of this page. This is a generic welcome message, press the buttons below the navigate trough the elements of this page. This is a generic welcome message, press the buttons below the navigate trough the elements of this page. This is a generic welcome message, press the buttons below the navigate trough the elements of this page. This is a generic welcome message, press the buttons below the navigate trough the elements of this page. </t>
-  </si>
-  <si>
-    <t>This is the second step. This is a generic welcome message, press the buttons below the navigate trough the elements of this page.  This is a generic welcome message, press the buttons below the navigate trough the elements of this page.  This is a generic welcome message, press the buttons below the navigate trough the elements of this page. This is a generic welcome message, press the buttons below the navigate trough the elements of this page. This is a generic welcome message, press the buttons below the navigate trough the elements of this page. This is a generic welcome message, press the buttons below the navigate trough the elements of this page. .</t>
   </si>
   <si>
     <t>#page_uploadData-sidebar</t>
@@ -221,12 +206,34 @@
     <t>Normally at the top of every module, there is an Introduction to the topic or functionality that is relevant to that module. &lt;br&gt;&lt;br&gt;
 &lt;i&gt;Tip:To expand/collade press the plus button at the right hand side of the bar. &lt;/i&gt;</t>
   </si>
+  <si>
+    <t xml:space="preserve">Here you have the options to read the correct format of the csv. </t>
+  </si>
+  <si>
+    <t>#page_uploadData-data_table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is highly recommended to download this csv template. You can do so by pressing this button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">After you input your own data, you can find and upload your file pressing this button. </t>
+  </si>
+  <si>
+    <t>If everything goes correctly, your data will show up in a table here. Once it shows correctly, press the "Calculate" tab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Upload Data Module &lt;/b&gt; &lt;br&gt;
+You can upload your own csv file with your data. Note that the format of the columns is very specific. Continue to get a walk through some of the features. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">And that’s it for the upload data module. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,6 +245,13 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -284,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -297,6 +311,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -693,7 +716,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -701,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -710,7 +733,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -718,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -727,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -735,7 +758,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -744,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -761,7 +784,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -778,7 +801,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -795,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -806,13 +829,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -823,13 +846,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -837,16 +860,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -860,10 +883,10 @@
         <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -871,16 +894,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -888,16 +911,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -905,16 +928,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -927,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,7 +964,7 @@
     <col min="6" max="256" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -958,226 +981,135 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="E14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1202,13 +1134,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,10 +1148,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1227,10 +1159,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,10 +1170,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1249,10 +1181,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1260,10 +1192,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>